<commit_message>
small fixes - mergeStrategy for artifact, ihc assay pointer corr to avail_assays and fixed uhc template example test protocol id to "ihc_..test"
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E686FA82-BAC0-1A44-BFE8-EB4C466955CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1E0F92-5A4B-6449-9D93-151C69B08AEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,9 +472,6 @@
     <t>Percentage fibrosis</t>
   </si>
   <si>
-    <t>E4412</t>
-  </si>
-  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
@@ -509,6 +506,9 @@
   </si>
   <si>
     <t>/path/to/hande.tiff</t>
+  </si>
+  <si>
+    <t>ihc_test_trial</t>
   </si>
 </sst>
 </file>
@@ -610,11 +610,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L11" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -970,22 +970,22 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -995,7 +995,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1018,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1041,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1064,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1087,7 +1087,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1110,7 +1110,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1133,7 +1133,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1202,7 +1202,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1225,7 +1225,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1248,7 +1248,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1264,26 +1264,26 @@
       <c r="O13" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1336,46 +1336,46 @@
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="4">
+      <c r="E17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="3">
+        <v>80</v>
+      </c>
+      <c r="G17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="4">
+      <c r="H17" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="I17" s="3">
         <v>80</v>
       </c>
-      <c r="G17" s="4">
+      <c r="J17" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="K17" s="3">
         <v>1</v>
       </c>
-      <c r="H17" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="I17" s="4">
+      <c r="L17" s="3">
         <v>80</v>
       </c>
-      <c r="J17" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="K17" s="4">
+      <c r="M17" s="3">
+        <v>80</v>
+      </c>
+      <c r="N17" s="3">
         <v>1</v>
       </c>
-      <c r="L17" s="4">
-        <v>80</v>
-      </c>
-      <c r="M17" s="4">
-        <v>80</v>
-      </c>
-      <c r="N17" s="4">
-        <v>1</v>
-      </c>
-      <c r="O17" s="4">
+      <c r="O17" s="3">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
.TIFF -> .QPTIFF support
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9A84A3-8316-6042-9F65-57B64AF4BAF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="37300" windowHeight="19320"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IHC" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -99,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -138,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -151,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -164,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -190,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -203,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -216,7 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -230,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -243,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0">
+    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -256,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -269,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -282,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -295,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0">
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -308,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J17" authorId="0">
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -592,16 +593,16 @@
     <t>test_prism_trial_id</t>
   </si>
   <si>
-    <t>path/to/image1.tiff</t>
-  </si>
-  <si>
-    <t>path/to/image2.tiff</t>
+    <t>path/to/image1.qptiff</t>
+  </si>
+  <si>
+    <t>path/to/image2.qptiff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -734,6 +735,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1025,11 +1029,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1054,7 +1058,7 @@
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1072,7 +1076,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1090,7 +1094,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1108,7 +1112,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1126,7 +1130,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1144,7 +1148,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1162,7 +1166,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1180,7 +1184,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1198,7 +1202,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1216,7 +1220,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1234,7 +1238,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1252,7 +1256,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1270,7 +1274,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2366,23 +2370,23 @@
     <mergeCell ref="D16:J16"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Bond RX,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D217">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D217" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"positive,negative,no_call"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2392,7 +2396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2402,17 +2406,17 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2423,7 +2427,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2437,7 +2441,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2451,7 +2455,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2465,7 +2469,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2479,7 +2483,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2490,7 +2494,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2501,7 +2505,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2512,7 +2516,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2523,7 +2527,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -2534,7 +2538,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
@@ -2545,7 +2549,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
@@ -2556,7 +2560,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -2567,7 +2571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
@@ -2597,7 +2601,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
@@ -2689,7 +2693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2699,7 +2703,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Support .QPTIFF & .SVS file types
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9A84A3-8316-6042-9F65-57B64AF4BAF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0499EA95-E7A4-A242-84A8-D2C12EA43CD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IHC" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,6 @@
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -240,7 +232,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates whether the marker is considered positive by clinical trial guidelines (if applicable).</t>
+          <t>Path to a file on a user's computer.
+In .svs format</t>
         </r>
       </text>
     </comment>
@@ -253,7 +246,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells.</t>
+          <t>Path to a file on a user's computer.
+In .qptiff format</t>
         </r>
       </text>
     </comment>
@@ -266,7 +260,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells.</t>
+          <t>Indicates whether the marker is considered positive by clinical trial guidelines (if applicable).</t>
         </r>
       </text>
     </comment>
@@ -279,7 +273,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells.</t>
+          <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells.</t>
         </r>
       </text>
     </comment>
@@ -292,7 +286,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage.</t>
+          <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells.</t>
         </r>
       </text>
     </comment>
@@ -305,11 +299,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>A semiquantitative approach used to assign score to tumor samples based on marker staining intensity (0, 1+, 2+, or 3+) for each cell in a fixed field.</t>
         </r>
       </text>
     </comment>
-    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="L17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -327,7 +347,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="94">
   <si>
     <t>#t</t>
   </si>
@@ -380,7 +400,7 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>Chromogenic IHC</t>
+    <t>Chromogenic IHC (please specify one score/metric)</t>
   </si>
   <si>
     <t>#h</t>
@@ -392,7 +412,13 @@
     <t>Cimac id</t>
   </si>
   <si>
-    <t>Ihc image</t>
+    <t>Ihc image (tiff)</t>
+  </si>
+  <si>
+    <t>Ihc image (svs)</t>
+  </si>
+  <si>
+    <t>Ihc image (qptiff)</t>
   </si>
   <si>
     <t>Marker positive</t>
@@ -497,7 +523,7 @@
     <t>Path to a file on a user's computer.</t>
   </si>
   <si>
-    <t>Section 'Chromogenic IHC' of tab 'IHC'</t>
+    <t>Section 'Chromogenic IHC (please specify one score/metric)' of tab 'IHC'</t>
   </si>
   <si>
     <t>Indicates whether the marker is considered positive by clinical trial guidelines (if applicable).</t>
@@ -569,6 +595,9 @@
     <t>no_call</t>
   </si>
   <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
     <t>XYZ</t>
   </si>
   <si>
@@ -578,9 +607,6 @@
     <t>#12345</t>
   </si>
   <si>
-    <t>100:5</t>
-  </si>
-  <si>
     <t>54c</t>
   </si>
   <si>
@@ -590,20 +616,26 @@
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>test_prism_trial_id</t>
+    <t>path/to/image1.tiff</t>
+  </si>
+  <si>
+    <t>path/to/image2.tiff</t>
+  </si>
+  <si>
+    <t>path/to/image1.svs</t>
+  </si>
+  <si>
+    <t>path/to/image2.svs</t>
   </si>
   <si>
     <t>path/to/image1.qptiff</t>
-  </si>
-  <si>
-    <t>path/to/image2.qptiff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -630,6 +662,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -702,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -716,7 +755,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -726,6 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,9 +829,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -819,14 +859,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -854,6 +911,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1030,19 +1104,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J217"/>
+  <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1057,8 +1131,10 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1066,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1075,8 +1151,10 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1084,7 +1162,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1093,8 +1171,10 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1102,7 +1182,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1111,8 +1191,10 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1120,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1129,8 +1211,10 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1138,7 +1222,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1147,8 +1231,10 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1156,7 +1242,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1165,8 +1251,10 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1174,7 +1262,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1183,8 +1271,10 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1192,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1201,8 +1291,10 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1210,7 +1302,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1219,8 +1311,10 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1228,7 +1322,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1237,16 +1331,18 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>83</v>
+      <c r="C12" s="5">
+        <v>4.1701388888888884</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1255,8 +1351,10 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1273,8 +1371,10 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1382,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1291,23 +1391,27 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1338,102 +1442,120 @@
       <c r="J17" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="C19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19">
+        <v>90</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19">
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -2365,9 +2487,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:L16"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2386,7 +2508,7 @@
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D217" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F217" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"positive,negative,no_call"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2397,7 +2519,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E26"/>
+  <dimension ref="B1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2408,12 +2530,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2421,10 +2543,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2432,13 +2554,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2446,13 +2568,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2460,13 +2582,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2474,13 +2596,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2488,10 +2610,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2499,10 +2621,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2510,10 +2632,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2521,10 +2643,10 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2532,10 +2654,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2543,10 +2665,10 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2554,10 +2676,10 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2565,15 +2687,15 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -2581,13 +2703,13 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -2595,20 +2717,26 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
@@ -2616,19 +2744,10 @@
       <c r="D20" t="s">
         <v>57</v>
       </c>
-      <c r="E20" t="s">
+    </row>
+    <row r="21" spans="2:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
@@ -2636,10 +2755,13 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
         <v>59</v>
       </c>
-      <c r="D22" t="s">
-        <v>61</v>
+      <c r="E22" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
@@ -2647,7 +2769,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
         <v>62</v>
@@ -2658,7 +2780,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
         <v>63</v>
@@ -2669,10 +2791,10 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
         <v>64</v>
-      </c>
-      <c r="D25" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
@@ -2680,10 +2802,32 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
         <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2717,54 +2861,54 @@
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
anyOf: TIFF, QPTIFF, SVS
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0499EA95-E7A4-A242-84A8-D2C12EA43CD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15724E73-62F4-1A43-95F0-33B0CD9630E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,12 +214,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.
-In .tiff format</t>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .tiff format</t>
         </r>
       </text>
     </comment>
@@ -347,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="91">
   <si>
     <t>#t</t>
   </si>
@@ -620,22 +629,13 @@
   </si>
   <si>
     <t>path/to/image2.tiff</t>
-  </si>
-  <si>
-    <t>path/to/image1.svs</t>
-  </si>
-  <si>
-    <t>path/to/image2.svs</t>
-  </si>
-  <si>
-    <t>path/to/image1.qptiff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,6 +669,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -762,10 +768,10 @@
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1120,19 +1126,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1395,21 +1401,21 @@
       <c r="L14" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1459,12 +1465,7 @@
       <c r="C18" t="s">
         <v>89</v>
       </c>
-      <c r="D18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>93</v>
-      </c>
+      <c r="E18" s="8"/>
       <c r="F18" t="s">
         <v>79</v>
       </c>
@@ -1482,12 +1483,8 @@
       <c r="C19" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>93</v>
-      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
       <c r="F19" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
tests for all supported extensions
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D2EF0E-A1DB-C64A-B93D-00089FD5759A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFF007A-5891-684D-AFA9-DAC92C771A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="93">
   <si>
     <t>#t</t>
   </si>
@@ -585,7 +585,19 @@
     <t>path/to/image1.tif</t>
   </si>
   <si>
-    <t>path/to/image2.tif</t>
+    <t>CTTTPP122.00</t>
+  </si>
+  <si>
+    <t>path/to/image2.tiff</t>
+  </si>
+  <si>
+    <t>CTTTPP123.00</t>
+  </si>
+  <si>
+    <t>path/to/image3.svs</t>
+  </si>
+  <si>
+    <t>path/to/image4.qptiff</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1380,7 +1392,7 @@
         <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s">
         <v>79</v>
@@ -1393,10 +1405,34 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21">
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
IHC template update to support multi file-format GCS-URIs (#263)
* update ihc template with 'template_comment'

* gcs_uri_format update

* bump __version__ = '0.13.4'

* update docs

* address comments

* tests for all supported extensions
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -1,40 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFF007A-5891-684D-AFA9-DAC92C771A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="37300" windowHeight="19320"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IHC" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -99,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -138,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -151,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -164,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -190,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -203,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -216,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -226,11 +219,11 @@
             <family val="2"/>
           </rPr>
           <t>Path to a file on a user's computer.
-In .tiff format</t>
+In one of .tiff .tif .qptiff .svs formats.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -243,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0">
+    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -256,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -269,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -282,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -295,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0">
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -308,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J17" authorId="0">
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -326,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="93">
   <si>
     <t>#t</t>
   </si>
@@ -379,7 +372,7 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>Chromogenic IHC</t>
+    <t>Chromogenic IHC (please specify one score/metric)</t>
   </si>
   <si>
     <t>#h</t>
@@ -496,7 +489,7 @@
     <t>Path to a file on a user's computer.</t>
   </si>
   <si>
-    <t>Section 'Chromogenic IHC' of tab 'IHC'</t>
+    <t>Section 'Chromogenic IHC (please specify one score/metric)' of tab 'IHC'</t>
   </si>
   <si>
     <t>Indicates whether the marker is considered positive by clinical trial guidelines (if applicable).</t>
@@ -568,6 +561,9 @@
     <t>no_call</t>
   </si>
   <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
     <t>XYZ</t>
   </si>
   <si>
@@ -577,9 +573,6 @@
     <t>#12345</t>
   </si>
   <si>
-    <t>100:5</t>
-  </si>
-  <si>
     <t>54c</t>
   </si>
   <si>
@@ -589,20 +582,29 @@
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>path/to/image1.tiff</t>
+    <t>path/to/image1.tif</t>
+  </si>
+  <si>
+    <t>CTTTPP122.00</t>
   </si>
   <si>
     <t>path/to/image2.tiff</t>
+  </si>
+  <si>
+    <t>CTTTPP123.00</t>
+  </si>
+  <si>
+    <t>path/to/image3.svs</t>
+  </si>
+  <si>
+    <t>path/to/image4.qptiff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,12 +624,6 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -701,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -715,13 +711,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -734,6 +729,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -785,9 +783,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -815,14 +813,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -850,6 +865,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1025,36 +1057,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1094,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1072,7 +1104,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1090,7 +1122,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1108,7 +1140,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1126,7 +1158,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1144,7 +1176,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1152,7 +1184,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1162,7 +1194,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1170,7 +1202,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1180,7 +1212,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1188,7 +1220,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1198,7 +1230,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1206,7 +1238,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1216,7 +1248,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1224,7 +1256,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1234,15 +1266,15 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>83</v>
+      <c r="C12" s="5">
+        <v>4.1701388888888884</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1252,7 +1284,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1270,7 +1302,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1289,19 +1321,19 @@
       <c r="J14" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1339,11 +1371,11 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" t="s">
         <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
         <v>77</v>
@@ -1356,7 +1388,7 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" t="s">
         <v>86</v>
       </c>
       <c r="C19" t="s">
@@ -1373,10 +1405,34 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21">
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -2366,23 +2422,23 @@
     <mergeCell ref="D16:J16"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Bond RX,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D217">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D217" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"positive,negative,no_call"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2392,7 +2448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2402,17 +2458,17 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2423,7 +2479,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2437,7 +2493,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2451,7 +2507,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2465,7 +2521,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2479,7 +2535,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2490,7 +2546,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2501,7 +2557,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2512,7 +2568,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2523,7 +2579,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -2534,7 +2590,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
@@ -2545,7 +2601,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
@@ -2556,7 +2612,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -2567,7 +2623,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
@@ -2597,7 +2653,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" ht="48" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
@@ -2689,7 +2745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2699,7 +2755,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
added intenstiy and % expression
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFF007A-5891-684D-AFA9-DAC92C771A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DCF029-A608-6447-BF26-8458B3409680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -245,7 +245,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells.</t>
+          <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells. (0-1)</t>
         </r>
       </text>
     </comment>
@@ -258,7 +258,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells.</t>
+          <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells. (0-1)</t>
         </r>
       </text>
     </comment>
@@ -271,7 +271,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells.</t>
+          <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells. (0-1)</t>
         </r>
       </text>
     </comment>
@@ -284,7 +284,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage.</t>
+          <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage. (0-1)</t>
         </r>
       </text>
     </comment>
@@ -297,11 +297,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>A semiquantitative approach used to assign score to tumor samples based on marker staining intensity (0, 1+, 2+, or 3+) for each cell in a fixed field.</t>
+          <t>A measure of the intensity or brightness of the protein. (0-3)</t>
         </r>
       </text>
     </comment>
     <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A percentage of the relevant cells considered positive. (0-100)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A summation of the percentage of area stained at each intensity level multiplied by the weighted intensity. (0-300)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -319,7 +345,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="97">
   <si>
     <t>#t</t>
   </si>
@@ -402,6 +428,12 @@
     <t>Positive inflammatory cell area</t>
   </si>
   <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>% expression</t>
+  </si>
+  <si>
     <t>H score</t>
   </si>
   <si>
@@ -501,22 +533,28 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells.</t>
-  </si>
-  <si>
-    <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells.</t>
-  </si>
-  <si>
-    <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells.</t>
-  </si>
-  <si>
-    <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage.</t>
+    <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells. (0-1)</t>
+  </si>
+  <si>
+    <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells. (0-1)</t>
+  </si>
+  <si>
+    <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells. (0-1)</t>
+  </si>
+  <si>
+    <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage. (0-1)</t>
+  </si>
+  <si>
+    <t>A measure of the intensity or brightness of the protein. (0-3)</t>
+  </si>
+  <si>
+    <t>A percentage of the relevant cells considered positive. (0-100)</t>
   </si>
   <si>
     <t>Integer</t>
   </si>
   <si>
-    <t>A semiquantitative approach used to assign score to tumor samples based on marker staining intensity (0, 1+, 2+, or 3+) for each cell in a fixed field.</t>
+    <t>A summation of the percentage of area stained at each intensity level multiplied by the weighted intensity. (0-300)</t>
   </si>
   <si>
     <t>A text comment regarding this slide.</t>
@@ -579,22 +617,22 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
+    <t>path/to/image1.tif</t>
+  </si>
+  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>path/to/image1.tif</t>
+    <t>path/to/image2.tiff</t>
   </si>
   <si>
     <t>CTTTPP122.00</t>
   </si>
   <si>
-    <t>path/to/image2.tiff</t>
+    <t>path/to/image3.svs</t>
   </si>
   <si>
     <t>CTTTPP123.00</t>
-  </si>
-  <si>
-    <t>path/to/image3.svs</t>
   </si>
   <si>
     <t>path/to/image4.qptiff</t>
@@ -604,7 +642,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,6 +663,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -697,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -711,15 +756,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="46" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J217"/>
+  <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1070,23 +1116,25 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1094,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1103,8 +1151,10 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1112,7 +1162,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1121,8 +1171,10 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1130,7 +1182,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1139,8 +1191,10 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1148,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1157,8 +1211,10 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1166,7 +1222,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1175,8 +1231,10 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1184,7 +1242,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1193,8 +1251,10 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1202,7 +1262,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1211,8 +1271,10 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1220,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1229,8 +1291,10 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1238,7 +1302,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1247,8 +1311,10 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1256,7 +1322,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1265,15 +1331,17 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>4.1701388888888884</v>
       </c>
       <c r="D12" s="2"/>
@@ -1283,15 +1351,17 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
         <v>0.28125</v>
       </c>
       <c r="D13" s="2"/>
@@ -1301,8 +1371,10 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1310,7 +1382,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1319,23 +1391,27 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1366,126 +1442,180 @@
       <c r="J17" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18">
+      <c r="B18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="8">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8">
+        <v>0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19">
+      <c r="B19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8">
+        <v>1</v>
+      </c>
+      <c r="J19" s="8">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20">
+      <c r="B20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8">
+        <v>2</v>
+      </c>
+      <c r="J20" s="8">
+        <v>40</v>
+      </c>
+      <c r="K20">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21">
+      <c r="B21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="8">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8">
+        <v>3</v>
+      </c>
+      <c r="J21" s="8">
+        <v>100</v>
+      </c>
+      <c r="K21">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -2417,28 +2547,28 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:L1"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D16:L16"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations disablePrompts="1" count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{06A8DF5B-32CB-064A-A97D-2B9E89AE8172}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{B7198C28-CA0E-2E4B-8A2D-85AE4EFC8C2A}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{C844F8AF-CE33-3847-BB83-FF4A3B4EF3E2}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{6D155AAA-6FFE-BF4F-BD65-58F04B8F16A4}">
       <formula1>"Bond RX,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13" xr:uid="{98E2AE1D-213F-624A-9859-3797A7B1A639}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D217" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22:D217" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"positive,negative,no_call"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2449,7 +2579,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E26"/>
+  <dimension ref="B1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2460,12 +2590,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2473,10 +2603,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2484,13 +2614,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2498,13 +2628,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2512,13 +2642,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2526,13 +2656,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2540,10 +2670,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2551,10 +2681,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2562,10 +2692,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2573,10 +2703,10 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2584,10 +2714,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2595,10 +2725,10 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2606,10 +2736,10 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2617,15 +2747,15 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -2633,13 +2763,13 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -2647,15 +2777,15 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="48" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
@@ -2663,13 +2793,13 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
@@ -2677,10 +2807,10 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
@@ -2688,10 +2818,10 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
@@ -2699,10 +2829,10 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -2710,10 +2840,10 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
@@ -2721,10 +2851,10 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
@@ -2732,10 +2862,32 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2774,49 +2926,49 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated IHC template (#276)
* added intenstiy and % expression

* update docs

* bump __version__ = '0.14.9'

Co-authored-by: Jacob Lurye <lurye.jacob@gmail.com>
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFF007A-5891-684D-AFA9-DAC92C771A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DCF029-A608-6447-BF26-8458B3409680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -245,7 +245,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells.</t>
+          <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells. (0-1)</t>
         </r>
       </text>
     </comment>
@@ -258,7 +258,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells.</t>
+          <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells. (0-1)</t>
         </r>
       </text>
     </comment>
@@ -271,7 +271,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells.</t>
+          <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells. (0-1)</t>
         </r>
       </text>
     </comment>
@@ -284,7 +284,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage.</t>
+          <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage. (0-1)</t>
         </r>
       </text>
     </comment>
@@ -297,11 +297,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>A semiquantitative approach used to assign score to tumor samples based on marker staining intensity (0, 1+, 2+, or 3+) for each cell in a fixed field.</t>
+          <t>A measure of the intensity or brightness of the protein. (0-3)</t>
         </r>
       </text>
     </comment>
     <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A percentage of the relevant cells considered positive. (0-100)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A summation of the percentage of area stained at each intensity level multiplied by the weighted intensity. (0-300)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -319,7 +345,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="97">
   <si>
     <t>#t</t>
   </si>
@@ -402,6 +428,12 @@
     <t>Positive inflammatory cell area</t>
   </si>
   <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>% expression</t>
+  </si>
+  <si>
     <t>H score</t>
   </si>
   <si>
@@ -501,22 +533,28 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells.</t>
-  </si>
-  <si>
-    <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells.</t>
-  </si>
-  <si>
-    <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells.</t>
-  </si>
-  <si>
-    <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage.</t>
+    <t>Tumor Proportion Score (TPS) is the percentage of viable tumor cells showing marker staining relative to all viable tumor cells. (0-1)</t>
+  </si>
+  <si>
+    <t>Combined Positive Score (CPS) is the percentage of marker staining cells (tumor cells and cells that are non-tumor) relative to all viable tumor cells. (0-1)</t>
+  </si>
+  <si>
+    <t>Percentage of inflammatory cells (non-tumor cells) showing marker staining relative to all inflammatory cells. (0-1)</t>
+  </si>
+  <si>
+    <t>Area of PD-L1+ Inflammatory Cells over the area of TSI + IT as a percentage. (0-1)</t>
+  </si>
+  <si>
+    <t>A measure of the intensity or brightness of the protein. (0-3)</t>
+  </si>
+  <si>
+    <t>A percentage of the relevant cells considered positive. (0-100)</t>
   </si>
   <si>
     <t>Integer</t>
   </si>
   <si>
-    <t>A semiquantitative approach used to assign score to tumor samples based on marker staining intensity (0, 1+, 2+, or 3+) for each cell in a fixed field.</t>
+    <t>A summation of the percentage of area stained at each intensity level multiplied by the weighted intensity. (0-300)</t>
   </si>
   <si>
     <t>A text comment regarding this slide.</t>
@@ -579,22 +617,22 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
+    <t>path/to/image1.tif</t>
+  </si>
+  <si>
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>path/to/image1.tif</t>
+    <t>path/to/image2.tiff</t>
   </si>
   <si>
     <t>CTTTPP122.00</t>
   </si>
   <si>
-    <t>path/to/image2.tiff</t>
+    <t>path/to/image3.svs</t>
   </si>
   <si>
     <t>CTTTPP123.00</t>
-  </si>
-  <si>
-    <t>path/to/image3.svs</t>
   </si>
   <si>
     <t>path/to/image4.qptiff</t>
@@ -604,7 +642,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,6 +663,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -697,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -711,15 +756,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="46" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J217"/>
+  <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1070,23 +1116,25 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1094,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1103,8 +1151,10 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1112,7 +1162,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1121,8 +1171,10 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1130,7 +1182,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1139,8 +1191,10 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1148,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1157,8 +1211,10 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1166,7 +1222,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1175,8 +1231,10 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1184,7 +1242,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1193,8 +1251,10 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1202,7 +1262,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1211,8 +1271,10 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1220,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1229,8 +1291,10 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1238,7 +1302,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1247,8 +1311,10 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1256,7 +1322,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1265,15 +1331,17 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>4.1701388888888884</v>
       </c>
       <c r="D12" s="2"/>
@@ -1283,15 +1351,17 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
         <v>0.28125</v>
       </c>
       <c r="D13" s="2"/>
@@ -1301,8 +1371,10 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1310,7 +1382,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1319,23 +1391,27 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1366,126 +1442,180 @@
       <c r="J17" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18">
+      <c r="B18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="8">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8">
+        <v>0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19">
+      <c r="B19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8">
+        <v>1</v>
+      </c>
+      <c r="J19" s="8">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20">
+      <c r="B20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8">
+        <v>2</v>
+      </c>
+      <c r="J20" s="8">
+        <v>40</v>
+      </c>
+      <c r="K20">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21">
+      <c r="B21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="8">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8">
+        <v>3</v>
+      </c>
+      <c r="J21" s="8">
+        <v>100</v>
+      </c>
+      <c r="K21">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -2417,28 +2547,28 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:L1"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D16:L16"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations disablePrompts="1" count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{06A8DF5B-32CB-064A-A97D-2B9E89AE8172}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{B7198C28-CA0E-2E4B-8A2D-85AE4EFC8C2A}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{C844F8AF-CE33-3847-BB83-FF4A3B4EF3E2}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{6D155AAA-6FFE-BF4F-BD65-58F04B8F16A4}">
       <formula1>"Bond RX,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13" xr:uid="{98E2AE1D-213F-624A-9859-3797A7B1A639}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D217" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22:D217" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"positive,negative,no_call"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2449,7 +2579,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E26"/>
+  <dimension ref="B1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2460,12 +2590,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2473,10 +2603,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2484,13 +2614,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2498,13 +2628,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2512,13 +2642,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2526,13 +2656,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2540,10 +2670,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2551,10 +2681,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2562,10 +2692,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2573,10 +2703,10 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2584,10 +2714,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2595,10 +2725,10 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2606,10 +2736,10 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -2617,15 +2747,15 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -2633,13 +2763,13 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -2647,15 +2777,15 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="48" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
@@ -2663,13 +2793,13 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
@@ -2677,10 +2807,10 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
@@ -2688,10 +2818,10 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
@@ -2699,10 +2829,10 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -2710,10 +2840,10 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
@@ -2721,10 +2851,10 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
@@ -2732,10 +2862,32 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2774,49 +2926,49 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add DFCI-Severgnini to Assay-creators
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DCF029-A608-6447-BF26-8458B3409680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B238A7-D4AB-F440-AE2D-76C08FEC2BB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="4900" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IHC" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -345,7 +345,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="98">
   <si>
     <t>#t</t>
   </si>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t>MD Anderson</t>
+  </si>
+  <si>
+    <t>DFCI-Severgnini</t>
   </si>
   <si>
     <t>Vectra 2.0</t>
@@ -665,11 +668,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -742,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -765,7 +767,6 @@
     <xf numFmtId="20" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1142,7 +1143,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1182,7 +1183,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1202,7 +1203,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1222,7 +1223,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1242,7 +1243,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1262,7 +1263,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1282,7 +1283,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1302,7 +1303,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1322,7 +1323,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1382,7 +1383,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1453,25 +1454,22 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="B18" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18">
         <v>0.67</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8">
+      <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
@@ -1482,25 +1480,22 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B19" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="8">
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19">
         <v>0.1</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8">
+      <c r="I19">
         <v>1</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19">
         <v>10</v>
       </c>
       <c r="K19">
@@ -1511,25 +1506,22 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B20" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="8">
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20">
         <v>0.1</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8">
+      <c r="I20">
         <v>2</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20">
         <v>40</v>
       </c>
       <c r="K20">
@@ -1540,25 +1532,22 @@
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="8">
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21">
         <v>0.2</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8">
+      <c r="I21">
         <v>3</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21">
         <v>100</v>
       </c>
       <c r="K21">
@@ -2551,25 +2540,25 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:L16"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{06A8DF5B-32CB-064A-A97D-2B9E89AE8172}">
-      <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{B7198C28-CA0E-2E4B-8A2D-85AE4EFC8C2A}">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{05F26F75-56B1-284E-AE31-789AEDA5907A}">
       <formula1>"Vectra 2.0,Hamamatsu"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{C844F8AF-CE33-3847-BB83-FF4A3B4EF3E2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{B415E49B-9379-CE4F-8695-4BCC25DB1580}">
       <formula1>"auto,manual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{6D155AAA-6FFE-BF4F-BD65-58F04B8F16A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{73D38955-BF7C-A244-87EC-F052708056C6}">
       <formula1>"Bond RX,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13" xr:uid="{98E2AE1D-213F-624A-9859-3797A7B1A639}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="C13" xr:uid="{619127CC-D52D-9C40-9F8A-2CA8E2DB665A}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22:D217" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D217" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"positive,negative,no_call"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{71DDED78-00EC-2043-9164-1CF770AEC527}">
+      <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2898,7 +2887,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:F5"/>
+  <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2929,16 +2918,16 @@
         <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -2946,16 +2935,16 @@
         <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
@@ -2963,12 +2952,17 @@
         <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test for integer like protocol id in ihc template
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DCF029-A608-6447-BF26-8458B3409680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFBECBD-2FD9-B44A-A7D4-98951D0D13FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -25,6 +25,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
+    <author>tc={DFEBFB27-270E-DA42-B6F7-71AD510C2E08}</author>
   </authors>
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -38,6 +39,15 @@
           </rPr>
           <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{DFEBFB27-270E-DA42-B6F7-71AD510C2E08}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    # testing integer protocol id
+</t>
       </text>
     </comment>
     <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
@@ -345,7 +355,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="96">
   <si>
     <t>#t</t>
   </si>
@@ -597,9 +607,6 @@
   </si>
   <si>
     <t>no_call</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id</t>
   </si>
   <si>
     <t>XYZ</t>
@@ -642,7 +649,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -670,6 +677,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -756,9 +769,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="46" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -766,6 +776,9 @@
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,6 +794,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Trukhanov, Pavel" id="{295596E3-C609-5F4E-AA95-2576DF890289}" userId="S::pavel_trukhanov@dfci.harvard.edu::dc7c4c00-d7fa-4037-b2d0-c05291f9522b" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1102,12 +1121,21 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C2" dT="2020-07-29T15:47:27.92" personId="{295596E3-C609-5F4E-AA95-2576DF890289}" id="{DFEBFB27-270E-DA42-B6F7-71AD510C2E08}">
+    <text xml:space="preserve"># testing integer protocol id
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1120,19 +1148,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1141,8 +1169,8 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>84</v>
+      <c r="C2" s="2">
+        <v>123</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1242,7 +1270,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1262,7 +1290,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1282,7 +1310,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1302,7 +1330,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1322,7 +1350,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1341,7 +1369,7 @@
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>4.1701388888888884</v>
       </c>
       <c r="D12" s="2"/>
@@ -1361,7 +1389,7 @@
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>0.28125</v>
       </c>
       <c r="D13" s="2"/>
@@ -1382,7 +1410,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1395,21 +1423,21 @@
       <c r="L14" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1453,25 +1481,25 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>0.67</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8">
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7">
         <v>0</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="7">
         <v>0</v>
       </c>
       <c r="K18">
@@ -1482,25 +1510,25 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>0.1</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7">
         <v>1</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="7">
         <v>10</v>
       </c>
       <c r="K19">
@@ -1511,25 +1539,25 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>0.1</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8">
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7">
         <v>2</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="7">
         <v>40</v>
       </c>
       <c r="K20">
@@ -1540,25 +1568,25 @@
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>0.2</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8">
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7">
         <v>3</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="7">
         <v>100</v>
       </c>
       <c r="K21">

</xml_diff>

<commit_message>
fix ihc gcs uri format lambda to not through errors on type mismatch
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFBECBD-2FD9-B44A-A7D4-98951D0D13FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ACB9A8-9DC5-884D-97EE-A5C7AFAA8F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23640" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IHC" sheetId="1" r:id="rId1"/>
@@ -355,7 +355,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="97">
   <si>
     <t>#t</t>
   </si>
@@ -643,13 +643,16 @@
   </si>
   <si>
     <t>path/to/image4.qptiff</t>
+  </si>
+  <si>
+    <t>Marker call</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -677,12 +680,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -717,7 +714,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -751,11 +748,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -778,6 +812,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1134,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1422,22 +1468,24 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -2577,7 +2625,7 @@
   <mergeCells count="3">
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:L16"/>
+    <mergeCell ref="E16:L16"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{06A8DF5B-32CB-064A-A97D-2B9E89AE8172}">

</xml_diff>

<commit_message>
Move multi-typing to DM instead of template
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -932,12 +932,12 @@
   <dimension ref="A1:L217"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
   </cols>
   <sheetData>
@@ -1351,7 +1351,7 @@
         <v>49</v>
       </c>
       <c r="E20" s="8" t="n">
-        <v>0.1</v>
+        <v>1.1</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
@@ -2429,9 +2429,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
   </cols>
   <sheetData>
@@ -2759,9 +2759,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Minimize warnings in tests; Update requirements
</commit_message>
<xml_diff>
--- a/template_examples/ihc_template.xlsx
+++ b/template_examples/ihc_template.xlsx
@@ -387,7 +387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="100">
   <si>
     <t xml:space="preserve">#title</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dilution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:100</t>
   </si>
   <si>
     <t xml:space="preserve">Incubation time</t>
@@ -931,11 +934,11 @@
   </sheetPr>
   <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
@@ -1166,8 +1169,8 @@
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="3" t="n">
-        <v>4.17013888888889</v>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1184,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>0.28125</v>
@@ -1204,10 +1207,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1221,17 +1224,17 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -1243,54 +1246,54 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="8" t="n">
         <v>0.67</v>
@@ -1310,16 +1313,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E19" s="8" t="n">
         <v>0.1</v>
@@ -1339,16 +1342,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E20" s="8" t="n">
         <v>0.1</v>
@@ -1368,19 +1371,19 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
@@ -1397,982 +1400,982 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +2432,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
@@ -2437,12 +2440,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2450,10 +2453,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2461,13 +2464,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2475,13 +2478,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2489,13 +2492,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2503,13 +2506,13 @@
         <v>10</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2517,10 +2520,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2528,10 +2531,10 @@
         <v>14</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2539,10 +2542,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2550,10 +2553,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2561,10 +2564,10 @@
         <v>18</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2572,169 +2575,169 @@
         <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2759,7 +2762,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
@@ -2779,7 +2782,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,37 +2799,37 @@
         <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>